<commit_message>
horas ocio dif tipos
</commit_message>
<xml_diff>
--- a/public/archivos/MPN.xlsx
+++ b/public/archivos/MPN.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23011"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23007"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lenovo\Desktop\10° Semestre\Integrador-Horarios\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{05E22D3D-BA31-4E2A-BE3B-626CDB263660}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{9A833F5E-D401-4EEC-8686-669F699182C6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11256" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="600" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="596" uniqueCount="130">
   <si>
     <t>cve_carrera</t>
   </si>
@@ -415,9 +415,6 @@
   </si>
   <si>
     <t>INTRODUCCION A LOS MATERIALES</t>
-  </si>
-  <si>
-    <t>LAB INTRODUCCION A LOS MATERIALES</t>
   </si>
   <si>
     <t>1007</t>
@@ -779,10 +776,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F121"/>
+  <dimension ref="A1:F120"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A102" workbookViewId="0">
-      <selection activeCell="I118" sqref="I118"/>
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
+      <selection activeCell="D42" sqref="D42"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="13.9"/>
@@ -3165,41 +3162,21 @@
         <v>121</v>
       </c>
       <c r="C119" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="D119" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="E119" s="3">
+        <v>1</v>
+      </c>
+      <c r="F119" s="3">
         <v>8</v>
       </c>
-      <c r="D119" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="E119" s="3">
-        <v>1</v>
-      </c>
-      <c r="F119" s="3">
-        <v>7</v>
-      </c>
     </row>
     <row r="120" spans="1:6" ht="12.75">
-      <c r="A120" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B120" s="3" t="s">
-        <v>121</v>
-      </c>
-      <c r="C120" s="3" t="s">
+      <c r="B120" s="1" t="s">
         <v>128</v>
-      </c>
-      <c r="D120" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E120" s="3">
-        <v>1</v>
-      </c>
-      <c r="F120" s="3">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="121" spans="1:6" ht="12.75">
-      <c r="B121" s="1" t="s">
-        <v>129</v>
       </c>
     </row>
   </sheetData>
@@ -3306,7 +3283,7 @@
         <v>30</v>
       </c>
       <c r="T3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="V3" t="s">
         <v>30</v>
@@ -3353,7 +3330,7 @@
         <v>57</v>
       </c>
       <c r="V4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="X4" t="s">
         <v>32</v>
@@ -3388,7 +3365,7 @@
         <v>45</v>
       </c>
       <c r="P5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="R5" t="s">
         <v>11</v>
@@ -3409,7 +3386,7 @@
         <v>11</v>
       </c>
       <c r="AE5" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="4:31">
@@ -3470,7 +3447,7 @@
         <v>63</v>
       </c>
       <c r="L7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N7" t="s">
         <v>76</v>
@@ -3479,7 +3456,7 @@
         <v>23</v>
       </c>
       <c r="R7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="T7" t="s">
         <v>63</v>
@@ -3488,10 +3465,10 @@
         <v>21</v>
       </c>
       <c r="X7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="Z7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="AB7" t="s">
         <v>13</v>

</xml_diff>